<commit_message>
changed oil preassure pin to A2
</commit_message>
<xml_diff>
--- a/miata_dash_v1.0/MS Excel.xlsx
+++ b/miata_dash_v1.0/MS Excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">light</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t xml:space="preserve">4 red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4</t>
   </si>
   <si>
     <t xml:space="preserve">       </t>
@@ -367,7 +391,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,9 +527,43 @@
         <v>15</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes to the excel formulas
</commit_message>
<xml_diff>
--- a/miata_dash_v1.0/MS Excel.xlsx
+++ b/miata_dash_v1.0/MS Excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t xml:space="preserve">light</t>
   </si>
@@ -94,17 +94,59 @@
     <t xml:space="preserve">A4</t>
   </si>
   <si>
+    <t xml:space="preserve">NORM OP TEMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOLTAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START VOLTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VOLT DIFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONVERT RATIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURRENT VOLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START VOLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMP</t>
+  </si>
+  <si>
     <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 GALLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL PSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 PSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -133,8 +175,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,13 +194,37 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF0101"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5EB91E"/>
+        <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0101"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF08B5FC"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -188,7 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,11 +271,63 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,7 +374,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FF08B5FC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -258,17 +384,17 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF5EB91E"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFFF0101"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -388,15 +514,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1026" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1026" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +548,7 @@
       <c r="B2" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -428,7 +559,7 @@
       <c r="B3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -461,7 +592,7 @@
       <c r="B6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="n">
@@ -472,7 +603,7 @@
       <c r="B7" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="n">
@@ -494,7 +625,7 @@
       <c r="B9" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="1" t="n">
@@ -505,7 +636,7 @@
       <c r="B10" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="n">
@@ -518,12 +649,12 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -561,10 +692,304 @@
         <v>23</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="1" t="s">
+      <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
+        <v>195</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="C21" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <f aca="false">C21-B21</f>
+        <v>4.87</v>
+      </c>
+      <c r="E21" s="11" t="n">
+        <f aca="false">(A21*0.01) / D21</f>
+        <v>0.40041067761807</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="B25" s="8" t="n">
+        <f aca="false">C21</f>
+        <v>10</v>
+      </c>
+      <c r="C25" s="12" t="n">
+        <f aca="false">B25-A25</f>
+        <v>4.87</v>
+      </c>
+      <c r="D25" s="13" t="n">
+        <f aca="false">(C25*100) * E21</f>
+        <v>195</v>
+      </c>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="n">
+        <v>0.83333</v>
+      </c>
+      <c r="C29" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" s="15" t="n">
+        <f aca="false">C29-B29</f>
+        <v>9.16667</v>
+      </c>
+      <c r="E29" s="11" t="n">
+        <f aca="false">(A29*0.01) / D29</f>
+        <v>0.00109090869421502</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B33" s="8" t="n">
+        <f aca="false">C29</f>
+        <v>10</v>
+      </c>
+      <c r="C33" s="12" t="n">
+        <f aca="false">B33-A33</f>
+        <v>5</v>
+      </c>
+      <c r="D33" s="13" t="n">
+        <f aca="false">(C33*100) * E29</f>
+        <v>0.54545434710751</v>
+      </c>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="B37" s="7" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="C37" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" s="15" t="n">
+        <f aca="false">C37-B37</f>
+        <v>4.87</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <f aca="false">(A37*0.01) / D37</f>
+        <v>0.0616016427104723</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="n">
+        <v>8.13</v>
+      </c>
+      <c r="B41" s="8" t="n">
+        <f aca="false">C37</f>
+        <v>10</v>
+      </c>
+      <c r="C41" s="12" t="n">
+        <f aca="false">B41-A41</f>
+        <v>1.87</v>
+      </c>
+      <c r="D41" s="13" t="n">
+        <f aca="false">(C41*100) * E37</f>
+        <v>11.5195071868583</v>
+      </c>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
made changes to excel file formulas
</commit_message>
<xml_diff>
--- a/miata_dash_v1.0/MS Excel.xlsx
+++ b/miata_dash_v1.0/MS Excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t xml:space="preserve">light</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulas for gauges</t>
   </si>
   <si>
     <t xml:space="preserve">NORM OP TEMP</t>
@@ -262,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,6 +284,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -514,10 +521,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -692,306 +699,315 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="C22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+      <c r="E22" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
         <v>195</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B23" s="8" t="n">
         <v>5.13</v>
       </c>
-      <c r="C21" s="8" t="n">
+      <c r="C23" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="D21" s="10" t="n">
-        <f aca="false">C21-B21</f>
+      <c r="D23" s="11" t="n">
+        <f aca="false">C23-B23</f>
         <v>4.87</v>
       </c>
-      <c r="E21" s="11" t="n">
-        <f aca="false">(A21*0.01) / D21</f>
+      <c r="E23" s="12" t="n">
+        <f aca="false">(A23*0.01) / D23</f>
         <v>0.40041067761807</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="9"/>
-    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="B27" s="9" t="n">
+        <f aca="false">C23</f>
+        <v>10</v>
+      </c>
+      <c r="C27" s="13" t="n">
+        <f aca="false">B27-A27</f>
+        <v>4.87</v>
+      </c>
+      <c r="D27" s="14" t="n">
+        <f aca="false">(C27*100) * E23</f>
+        <v>195</v>
+      </c>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="7" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="8" t="n">
+        <v>0.83333</v>
+      </c>
+      <c r="C31" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D31" s="16" t="n">
+        <f aca="false">C31-B31</f>
+        <v>9.16667</v>
+      </c>
+      <c r="E31" s="12" t="n">
+        <f aca="false">(A31*0.01) / D31</f>
+        <v>0.00109090869421502</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="B34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" s="9" t="n">
+        <f aca="false">C31</f>
+        <v>10</v>
+      </c>
+      <c r="C35" s="13" t="n">
+        <f aca="false">B35-A35</f>
+        <v>5</v>
+      </c>
+      <c r="D35" s="14" t="n">
+        <f aca="false">(C35*100) * E31</f>
+        <v>0.54545434710751</v>
+      </c>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B39" s="8" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="C39" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" s="16" t="n">
+        <f aca="false">C39-B39</f>
+        <v>1.17</v>
+      </c>
+      <c r="E39" s="12" t="n">
+        <f aca="false">(A39*0.01) / D39</f>
+        <v>0.256410256410256</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="B25" s="8" t="n">
-        <f aca="false">C21</f>
-        <v>10</v>
-      </c>
-      <c r="C25" s="12" t="n">
-        <f aca="false">B25-A25</f>
-        <v>4.87</v>
-      </c>
-      <c r="D25" s="13" t="n">
-        <f aca="false">(C25*100) * E21</f>
-        <v>195</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="C42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7" t="n">
-        <v>0.83333</v>
-      </c>
-      <c r="C29" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="D29" s="15" t="n">
-        <f aca="false">C29-B29</f>
-        <v>9.16667</v>
-      </c>
-      <c r="E29" s="11" t="n">
-        <f aca="false">(A29*0.01) / D29</f>
-        <v>0.00109090869421502</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B43" s="9" t="n">
+        <f aca="false">C39</f>
         <v>5</v>
       </c>
-      <c r="B33" s="8" t="n">
-        <f aca="false">C29</f>
-        <v>10</v>
-      </c>
-      <c r="C33" s="12" t="n">
-        <f aca="false">B33-A33</f>
-        <v>5</v>
-      </c>
-      <c r="D33" s="13" t="n">
-        <f aca="false">(C33*100) * E29</f>
-        <v>0.54545434710751</v>
-      </c>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="B37" s="7" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="C37" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="D37" s="15" t="n">
-        <f aca="false">C37-B37</f>
-        <v>4.87</v>
-      </c>
-      <c r="E37" s="11" t="n">
-        <f aca="false">(A37*0.01) / D37</f>
-        <v>0.0616016427104723</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="n">
-        <v>8.13</v>
-      </c>
-      <c r="B41" s="8" t="n">
-        <f aca="false">C37</f>
-        <v>10</v>
-      </c>
-      <c r="C41" s="12" t="n">
-        <f aca="false">B41-A41</f>
-        <v>1.87</v>
-      </c>
-      <c r="D41" s="13" t="n">
-        <f aca="false">(C41*100) * E37</f>
-        <v>11.5195071868583</v>
-      </c>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="16"/>
+      <c r="C43" s="13" t="n">
+        <f aca="false">B43-A43</f>
+        <v>1.9</v>
+      </c>
+      <c r="D43" s="14" t="n">
+        <f aca="false">(C43*100) * E39</f>
+        <v>48.7179487179487</v>
+      </c>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C20:D20"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
took sample data from gauges
</commit_message>
<xml_diff>
--- a/miata_dash_v1.0/MS Excel.xlsx
+++ b/miata_dash_v1.0/MS Excel.xlsx
@@ -286,7 +286,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,10 +521,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1004,6 +1004,46 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="17"/>
     </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="2" t="n">
+        <v>10.05</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="2" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="2" t="n">
+        <v>7.92</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="2" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="2" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C20:D20"/>

</xml_diff>